<commit_message>
minor edits to get genes present on the assembly
</commit_message>
<xml_diff>
--- a/docs/s_infantis_plasmid_annotation.xlsx
+++ b/docs/s_infantis_plasmid_annotation.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="s_infantis_plasmid_annotation" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">s_infantis_plasmid_annotation!$A$1:$N$6</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="1882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="1882">
   <si>
     <t xml:space="preserve">#Annotated with Bakta (v1.7.0): https://github.com/oschwengers/bakta</t>
   </si>
@@ -5749,12 +5750,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5865,19 +5862,19 @@
   </sheetPr>
   <dimension ref="A1:X294"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B295" activeCellId="0" sqref="B295"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="52.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="59.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.63"/>
@@ -5888,7 +5885,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="27.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.13"/>
@@ -5904,7 +5901,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -5953,10 +5950,10 @@
       <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="2" t="n">
         <v>1011</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -5988,10 +5985,10 @@
       <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="2" t="n">
         <v>3420</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="2" t="n">
         <v>3686</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -6029,10 +6026,10 @@
       <c r="B6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="n">
         <v>4366</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="2" t="n">
         <v>6246</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -6041,7 +6038,7 @@
       <c r="F6" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -6067,8 +6064,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -6077,10 +6074,10 @@
       <c r="B8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>8264</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="2" t="n">
         <v>9022</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -6118,10 +6115,10 @@
       <c r="B9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="2" t="n">
         <v>9004</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="2" t="n">
         <v>9432</v>
       </c>
       <c r="E9" s="0" t="s">
@@ -6159,10 +6156,10 @@
       <c r="B10" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="2" t="n">
         <v>9488</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>9997</v>
       </c>
       <c r="E10" s="0" t="s">
@@ -6244,10 +6241,10 @@
       <c r="B15" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="2" t="n">
         <v>14531</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="2" t="n">
         <v>14788</v>
       </c>
       <c r="E15" s="0" t="s">
@@ -6294,10 +6291,10 @@
       <c r="B16" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="2" t="n">
         <v>14789</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="2" t="n">
         <v>15121</v>
       </c>
       <c r="E16" s="0" t="s">
@@ -6347,10 +6344,10 @@
       <c r="B17" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="2" t="n">
         <v>15715</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="2" t="n">
         <v>16326</v>
       </c>
       <c r="E17" s="0" t="s">
@@ -6379,10 +6376,10 @@
       <c r="B18" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="2" t="n">
         <v>16625</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="2" t="n">
         <v>18847</v>
       </c>
       <c r="E18" s="0" t="s">
@@ -6423,10 +6420,10 @@
       <c r="B19" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="2" t="n">
         <v>18844</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="2" t="n">
         <v>20160</v>
       </c>
       <c r="E19" s="0" t="s">
@@ -6464,10 +6461,10 @@
       <c r="B20" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="2" t="n">
         <v>20164</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="2" t="n">
         <v>22473</v>
       </c>
       <c r="E20" s="0" t="s">
@@ -6505,10 +6502,10 @@
       <c r="B21" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="2" t="n">
         <v>22797</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="2" t="n">
         <v>23024</v>
       </c>
       <c r="E21" s="0" t="s">
@@ -6534,10 +6531,10 @@
       <c r="B22" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="2" t="n">
         <v>23156</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="2" t="n">
         <v>24181</v>
       </c>
       <c r="E22" s="0" t="s">
@@ -6575,10 +6572,10 @@
       <c r="B23" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="2" t="n">
         <v>24431</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="2" t="n">
         <v>24598</v>
       </c>
       <c r="E23" s="0" t="s">
@@ -6613,10 +6610,10 @@
       <c r="B24" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="2" t="n">
         <v>24585</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="2" t="n">
         <v>24914</v>
       </c>
       <c r="E24" s="0" t="s">
@@ -6651,8 +6648,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -6661,10 +6658,10 @@
       <c r="B26" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="2" t="n">
         <v>25544</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="2" t="n">
         <v>25891</v>
       </c>
       <c r="E26" s="0" t="s">
@@ -6673,7 +6670,7 @@
       <c r="F26" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>136</v>
       </c>
       <c r="H26" s="0" t="s">
@@ -6693,10 +6690,10 @@
       <c r="B27" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="2" t="n">
         <v>25860</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="2" t="n">
         <v>26147</v>
       </c>
       <c r="E27" s="0" t="s">
@@ -6728,8 +6725,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -6738,10 +6735,10 @@
       <c r="B29" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="2" t="n">
         <v>27199</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="2" t="n">
         <v>27462</v>
       </c>
       <c r="E29" s="0" t="s">
@@ -6779,10 +6776,10 @@
       <c r="B30" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="2" t="n">
         <v>27488</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="2" t="n">
         <v>27823</v>
       </c>
       <c r="E30" s="0" t="s">
@@ -6820,10 +6817,10 @@
       <c r="B31" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="2" t="n">
         <v>28611</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="2" t="n">
         <v>28895</v>
       </c>
       <c r="E31" s="0" t="s">
@@ -6867,10 +6864,10 @@
       <c r="B32" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="2" t="n">
         <v>28886</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="2" t="n">
         <v>29368</v>
       </c>
       <c r="E32" s="0" t="s">
@@ -6908,10 +6905,10 @@
       <c r="B33" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="2" t="n">
         <v>29744</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="2" t="n">
         <v>30109</v>
       </c>
       <c r="E33" s="0" t="s">
@@ -6937,8 +6934,8 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -6947,10 +6944,10 @@
       <c r="B35" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="2" t="n">
         <v>32034</v>
       </c>
-      <c r="D35" s="3" t="n">
+      <c r="D35" s="2" t="n">
         <v>32276</v>
       </c>
       <c r="E35" s="0" t="s">
@@ -6991,10 +6988,10 @@
       <c r="B36" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="2" t="n">
         <v>32263</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="2" t="n">
         <v>32505</v>
       </c>
       <c r="E36" s="0" t="s">
@@ -7032,10 +7029,10 @@
       <c r="B37" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="2" t="n">
         <v>32576</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="2" t="n">
         <v>33532</v>
       </c>
       <c r="E37" s="0" t="s">
@@ -7073,10 +7070,10 @@
       <c r="B38" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="2" t="n">
         <v>33591</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="2" t="n">
         <v>33803</v>
       </c>
       <c r="E38" s="0" t="s">
@@ -7114,10 +7111,10 @@
       <c r="B39" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="2" t="n">
         <v>33845</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="2" t="n">
         <v>34060</v>
       </c>
       <c r="E39" s="0" t="s">
@@ -7155,10 +7152,10 @@
       <c r="B40" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="2" t="n">
         <v>34512</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="2" t="n">
         <v>35660</v>
       </c>
       <c r="E40" s="0" t="s">
@@ -7167,7 +7164,7 @@
       <c r="F40" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>214</v>
       </c>
       <c r="H40" s="0" t="s">
@@ -7196,10 +7193,10 @@
       <c r="B41" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="2" t="n">
         <v>35792</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="2" t="n">
         <v>35871</v>
       </c>
       <c r="E41" s="0" t="s">
@@ -7216,10 +7213,10 @@
       <c r="B42" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="2" t="n">
         <v>35887</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="2" t="n">
         <v>36060</v>
       </c>
       <c r="E42" s="0" t="s">
@@ -7251,10 +7248,10 @@
       <c r="B43" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="2" t="n">
         <v>36103</v>
       </c>
-      <c r="D43" s="3" t="n">
+      <c r="D43" s="2" t="n">
         <v>36219</v>
       </c>
       <c r="E43" s="0" t="s">
@@ -7280,8 +7277,8 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -7290,10 +7287,10 @@
       <c r="B45" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="2" t="n">
         <v>36997</v>
       </c>
-      <c r="D45" s="3" t="n">
+      <c r="D45" s="2" t="n">
         <v>37242</v>
       </c>
       <c r="E45" s="0" t="s">
@@ -7313,8 +7310,8 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -7323,10 +7320,10 @@
       <c r="B47" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C47" s="2" t="n">
         <v>37521</v>
       </c>
-      <c r="D47" s="3" t="n">
+      <c r="D47" s="2" t="n">
         <v>37655</v>
       </c>
       <c r="E47" s="0" t="s">
@@ -7355,10 +7352,10 @@
       <c r="B48" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="3" t="n">
+      <c r="C48" s="2" t="n">
         <v>38204</v>
       </c>
-      <c r="D48" s="3" t="n">
+      <c r="D48" s="2" t="n">
         <v>38524</v>
       </c>
       <c r="E48" s="0" t="s">
@@ -7399,10 +7396,10 @@
       <c r="B49" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="3" t="n">
+      <c r="C49" s="2" t="n">
         <v>38569</v>
       </c>
-      <c r="D49" s="3" t="n">
+      <c r="D49" s="2" t="n">
         <v>39108</v>
       </c>
       <c r="E49" s="0" t="s">
@@ -7440,10 +7437,10 @@
       <c r="B50" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="3" t="n">
+      <c r="C50" s="2" t="n">
         <v>39133</v>
       </c>
-      <c r="D50" s="3" t="n">
+      <c r="D50" s="2" t="n">
         <v>41565</v>
       </c>
       <c r="E50" s="0" t="s">
@@ -7484,10 +7481,10 @@
       <c r="B51" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="3" t="n">
+      <c r="C51" s="2" t="n">
         <v>41582</v>
       </c>
-      <c r="D51" s="3" t="n">
+      <c r="D51" s="2" t="n">
         <v>42373</v>
       </c>
       <c r="E51" s="0" t="s">
@@ -7525,10 +7522,10 @@
       <c r="B52" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="3" t="n">
+      <c r="C52" s="2" t="n">
         <v>42406</v>
       </c>
-      <c r="D52" s="3" t="n">
+      <c r="D52" s="2" t="n">
         <v>42900</v>
       </c>
       <c r="E52" s="0" t="s">
@@ -7560,10 +7557,10 @@
       <c r="B53" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="D53" s="3" t="n">
+      <c r="D53" s="2" t="n">
         <v>43949</v>
       </c>
       <c r="E53" s="0" t="s">
@@ -7601,10 +7598,10 @@
       <c r="B54" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="3" t="n">
+      <c r="C54" s="2" t="n">
         <v>44110</v>
       </c>
-      <c r="D54" s="3" t="n">
+      <c r="D54" s="2" t="n">
         <v>44901</v>
       </c>
       <c r="E54" s="0" t="s">
@@ -7648,10 +7645,10 @@
       <c r="B55" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="3" t="n">
+      <c r="C55" s="2" t="n">
         <v>44929</v>
       </c>
-      <c r="D55" s="3" t="n">
+      <c r="D55" s="2" t="n">
         <v>45693</v>
       </c>
       <c r="E55" s="0" t="s">
@@ -7692,10 +7689,10 @@
       <c r="B56" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" s="2" t="n">
         <v>45908</v>
       </c>
-      <c r="D56" s="3" t="n">
+      <c r="D56" s="2" t="n">
         <v>46486</v>
       </c>
       <c r="E56" s="0" t="s">
@@ -7724,10 +7721,10 @@
       <c r="B57" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="3" t="n">
+      <c r="C57" s="2" t="n">
         <v>46552</v>
       </c>
-      <c r="D57" s="3" t="n">
+      <c r="D57" s="2" t="n">
         <v>46764</v>
       </c>
       <c r="E57" s="0" t="s">
@@ -7765,10 +7762,10 @@
       <c r="B58" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="3" t="n">
+      <c r="C58" s="2" t="n">
         <v>47040</v>
       </c>
-      <c r="D58" s="3" t="n">
+      <c r="D58" s="2" t="n">
         <v>47186</v>
       </c>
       <c r="E58" s="0" t="s">
@@ -7806,10 +7803,10 @@
       <c r="B59" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="3" t="n">
+      <c r="C59" s="2" t="n">
         <v>47212</v>
       </c>
-      <c r="D59" s="3" t="n">
+      <c r="D59" s="2" t="n">
         <v>48060</v>
       </c>
       <c r="E59" s="0" t="s">
@@ -7847,10 +7844,10 @@
       <c r="B60" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" s="2" t="n">
         <v>48135</v>
       </c>
-      <c r="D60" s="3" t="n">
+      <c r="D60" s="2" t="n">
         <v>48401</v>
       </c>
       <c r="E60" s="0" t="s">
@@ -7879,10 +7876,10 @@
       <c r="B61" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" s="2" t="n">
         <v>48630</v>
       </c>
-      <c r="D61" s="3" t="n">
+      <c r="D61" s="2" t="n">
         <v>49046</v>
       </c>
       <c r="E61" s="0" t="s">
@@ -7932,10 +7929,10 @@
       <c r="B62" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="3" t="n">
+      <c r="C62" s="2" t="n">
         <v>49043</v>
       </c>
-      <c r="D62" s="3" t="n">
+      <c r="D62" s="2" t="n">
         <v>49273</v>
       </c>
       <c r="E62" s="0" t="s">
@@ -7979,8 +7976,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -7989,10 +7986,10 @@
       <c r="B64" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="3" t="n">
+      <c r="C64" s="2" t="n">
         <v>49897</v>
       </c>
-      <c r="D64" s="3" t="n">
+      <c r="D64" s="2" t="n">
         <v>50115</v>
       </c>
       <c r="E64" s="0" t="s">
@@ -8039,10 +8036,10 @@
       <c r="B65" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="3" t="n">
+      <c r="C65" s="2" t="n">
         <v>50117</v>
       </c>
-      <c r="D65" s="3" t="n">
+      <c r="D65" s="2" t="n">
         <v>50422</v>
       </c>
       <c r="E65" s="0" t="s">
@@ -8086,10 +8083,10 @@
       <c r="B66" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="3" t="n">
+      <c r="C66" s="2" t="n">
         <v>50424</v>
       </c>
-      <c r="D66" s="3" t="n">
+      <c r="D66" s="2" t="n">
         <v>50714</v>
       </c>
       <c r="E66" s="0" t="s">
@@ -8127,10 +8124,10 @@
       <c r="B67" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="3" t="n">
+      <c r="C67" s="2" t="n">
         <v>50711</v>
       </c>
-      <c r="D67" s="3" t="n">
+      <c r="D67" s="2" t="n">
         <v>51340</v>
       </c>
       <c r="E67" s="0" t="s">
@@ -8153,8 +8150,8 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
@@ -8163,10 +8160,10 @@
       <c r="B69" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C69" s="2" t="n">
         <v>53160</v>
       </c>
-      <c r="D69" s="3" t="n">
+      <c r="D69" s="2" t="n">
         <v>53696</v>
       </c>
       <c r="E69" s="0" t="s">
@@ -8204,10 +8201,10 @@
       <c r="B70" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C70" s="3" t="n">
+      <c r="C70" s="2" t="n">
         <v>53749</v>
       </c>
-      <c r="D70" s="3" t="n">
+      <c r="D70" s="2" t="n">
         <v>54480</v>
       </c>
       <c r="E70" s="0" t="s">
@@ -8248,10 +8245,10 @@
       <c r="B71" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="3" t="n">
+      <c r="C71" s="2" t="n">
         <v>54491</v>
       </c>
-      <c r="D71" s="3" t="n">
+      <c r="D71" s="2" t="n">
         <v>57073</v>
       </c>
       <c r="E71" s="0" t="s">
@@ -8292,10 +8289,10 @@
       <c r="B72" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="3" t="n">
+      <c r="C72" s="2" t="n">
         <v>57230</v>
       </c>
-      <c r="D72" s="3" t="n">
+      <c r="D72" s="2" t="n">
         <v>58279</v>
       </c>
       <c r="E72" s="0" t="s">
@@ -8333,10 +8330,10 @@
       <c r="B73" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="3" t="n">
+      <c r="C73" s="2" t="n">
         <v>58981</v>
       </c>
-      <c r="D73" s="3" t="n">
+      <c r="D73" s="2" t="n">
         <v>59268</v>
       </c>
       <c r="E73" s="0" t="s">
@@ -8371,10 +8368,10 @@
       <c r="B74" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C74" s="3" t="n">
+      <c r="C74" s="2" t="n">
         <v>60049</v>
       </c>
-      <c r="D74" s="3" t="n">
+      <c r="D74" s="2" t="n">
         <v>60186</v>
       </c>
       <c r="E74" s="0" t="s">
@@ -8400,10 +8397,10 @@
       <c r="B75" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="3" t="n">
+      <c r="C75" s="2" t="n">
         <v>60751</v>
       </c>
-      <c r="D75" s="3" t="n">
+      <c r="D75" s="2" t="n">
         <v>61323</v>
       </c>
       <c r="E75" s="0" t="s">
@@ -8423,12 +8420,12 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
@@ -8437,10 +8434,10 @@
       <c r="B78" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="3" t="n">
+      <c r="C78" s="2" t="n">
         <v>63154</v>
       </c>
-      <c r="D78" s="3" t="n">
+      <c r="D78" s="2" t="n">
         <v>63651</v>
       </c>
       <c r="E78" s="0" t="s">
@@ -8472,10 +8469,10 @@
       <c r="B79" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="C79" s="3" t="n">
+      <c r="C79" s="2" t="n">
         <v>63635</v>
       </c>
-      <c r="D79" s="3" t="n">
+      <c r="D79" s="2" t="n">
         <v>63706</v>
       </c>
       <c r="E79" s="0" t="s">
@@ -8504,8 +8501,8 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
@@ -8514,10 +8511,10 @@
       <c r="B81" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C81" s="3" t="n">
+      <c r="C81" s="2" t="n">
         <v>65398</v>
       </c>
-      <c r="D81" s="3" t="n">
+      <c r="D81" s="2" t="n">
         <v>65823</v>
       </c>
       <c r="E81" s="0" t="s">
@@ -8555,10 +8552,10 @@
       <c r="B82" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C82" s="3" t="n">
+      <c r="C82" s="2" t="n">
         <v>65820</v>
       </c>
-      <c r="D82" s="3" t="n">
+      <c r="D82" s="2" t="n">
         <v>66539</v>
       </c>
       <c r="E82" s="0" t="s">
@@ -8590,8 +8587,8 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
@@ -8600,10 +8597,10 @@
       <c r="B84" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="3" t="n">
+      <c r="C84" s="2" t="n">
         <v>66974</v>
       </c>
-      <c r="D84" s="3" t="n">
+      <c r="D84" s="2" t="n">
         <v>67534</v>
       </c>
       <c r="E84" s="0" t="s">
@@ -8638,10 +8635,10 @@
       <c r="B85" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C85" s="3" t="n">
+      <c r="C85" s="2" t="n">
         <v>67657</v>
       </c>
-      <c r="D85" s="3" t="n">
+      <c r="D85" s="2" t="n">
         <v>68907</v>
       </c>
       <c r="E85" s="0" t="s">
@@ -8679,10 +8676,10 @@
       <c r="B86" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="3" t="n">
+      <c r="C86" s="2" t="n">
         <v>68916</v>
       </c>
-      <c r="D86" s="3" t="n">
+      <c r="D86" s="2" t="n">
         <v>71012</v>
       </c>
       <c r="E86" s="0" t="s">
@@ -8720,10 +8717,10 @@
       <c r="B87" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C87" s="3" t="n">
+      <c r="C87" s="2" t="n">
         <v>71386</v>
       </c>
-      <c r="D87" s="3" t="n">
+      <c r="D87" s="2" t="n">
         <v>72018</v>
       </c>
       <c r="E87" s="0" t="s">
@@ -8752,10 +8749,10 @@
       <c r="B88" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="3" t="n">
+      <c r="C88" s="2" t="n">
         <v>72318</v>
       </c>
-      <c r="D88" s="3" t="n">
+      <c r="D88" s="2" t="n">
         <v>72578</v>
       </c>
       <c r="E88" s="0" t="s">
@@ -8784,10 +8781,10 @@
       <c r="B89" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="3" t="n">
+      <c r="C89" s="2" t="n">
         <v>74522</v>
       </c>
-      <c r="D89" s="3" t="n">
+      <c r="D89" s="2" t="n">
         <v>74884</v>
       </c>
       <c r="E89" s="0" t="s">
@@ -8825,10 +8822,10 @@
       <c r="B90" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="3" t="n">
+      <c r="C90" s="2" t="n">
         <v>75013</v>
       </c>
-      <c r="D90" s="3" t="n">
+      <c r="D90" s="2" t="n">
         <v>75450</v>
       </c>
       <c r="E90" s="0" t="s">
@@ -8866,10 +8863,10 @@
       <c r="B91" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C91" s="3" t="n">
+      <c r="C91" s="2" t="n">
         <v>75949</v>
       </c>
-      <c r="D91" s="3" t="n">
+      <c r="D91" s="2" t="n">
         <v>76428</v>
       </c>
       <c r="E91" s="0" t="s">
@@ -8936,10 +8933,10 @@
       <c r="B93" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="3" t="n">
+      <c r="C93" s="2" t="n">
         <v>82006</v>
       </c>
-      <c r="D93" s="3" t="n">
+      <c r="D93" s="2" t="n">
         <v>82764</v>
       </c>
       <c r="E93" s="0" t="s">
@@ -8980,10 +8977,10 @@
       <c r="B94" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="3" t="n">
+      <c r="C94" s="2" t="n">
         <v>83078</v>
       </c>
-      <c r="D94" s="3" t="n">
+      <c r="D94" s="2" t="n">
         <v>83344</v>
       </c>
       <c r="E94" s="0" t="s">
@@ -9030,10 +9027,10 @@
       <c r="B95" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="C95" s="3" t="n">
+      <c r="C95" s="2" t="n">
         <v>83343</v>
       </c>
-      <c r="D95" s="3" t="n">
+      <c r="D95" s="2" t="n">
         <v>83479</v>
       </c>
       <c r="E95" s="0" t="s">
@@ -9062,10 +9059,10 @@
       <c r="B96" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="3" t="n">
+      <c r="C96" s="2" t="n">
         <v>83368</v>
       </c>
-      <c r="D96" s="3" t="n">
+      <c r="D96" s="2" t="n">
         <v>84177</v>
       </c>
       <c r="E96" s="0" t="s">
@@ -9106,10 +9103,10 @@
       <c r="B97" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="3" t="n">
+      <c r="C97" s="2" t="n">
         <v>84118</v>
       </c>
-      <c r="D97" s="3" t="n">
+      <c r="D97" s="2" t="n">
         <v>84420</v>
       </c>
       <c r="E97" s="0" t="s">
@@ -9138,8 +9135,8 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
@@ -9148,10 +9145,10 @@
       <c r="B99" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="3" t="n">
+      <c r="C99" s="2" t="n">
         <v>85035</v>
       </c>
-      <c r="D99" s="3" t="n">
+      <c r="D99" s="2" t="n">
         <v>86150</v>
       </c>
       <c r="E99" s="0" t="s">
@@ -9189,10 +9186,10 @@
       <c r="B100" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C100" s="3" t="n">
+      <c r="C100" s="2" t="n">
         <v>86738</v>
       </c>
-      <c r="D100" s="3" t="n">
+      <c r="D100" s="2" t="n">
         <v>87595</v>
       </c>
       <c r="E100" s="0" t="s">
@@ -9221,10 +9218,10 @@
       <c r="B101" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="3" t="n">
+      <c r="C101" s="2" t="n">
         <v>87997</v>
       </c>
-      <c r="D101" s="3" t="n">
+      <c r="D101" s="2" t="n">
         <v>88458</v>
       </c>
       <c r="E101" s="0" t="s">
@@ -9259,10 +9256,10 @@
       <c r="B102" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C102" s="3" t="n">
+      <c r="C102" s="2" t="n">
         <v>88455</v>
       </c>
-      <c r="D102" s="3" t="n">
+      <c r="D102" s="2" t="n">
         <v>88685</v>
       </c>
       <c r="E102" s="0" t="s">
@@ -9300,10 +9297,10 @@
       <c r="B103" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="3" t="n">
+      <c r="C103" s="2" t="n">
         <v>88997</v>
       </c>
-      <c r="D103" s="3" t="n">
+      <c r="D103" s="2" t="n">
         <v>89728</v>
       </c>
       <c r="E103" s="0" t="s">
@@ -9335,10 +9332,10 @@
       <c r="B104" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C104" s="3" t="n">
+      <c r="C104" s="2" t="n">
         <v>89694</v>
       </c>
-      <c r="D104" s="3" t="n">
+      <c r="D104" s="2" t="n">
         <v>89957</v>
       </c>
       <c r="E104" s="0" t="s">
@@ -9364,10 +9361,10 @@
       <c r="B105" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C105" s="3" t="n">
+      <c r="C105" s="2" t="n">
         <v>90430</v>
       </c>
-      <c r="D105" s="3" t="n">
+      <c r="D105" s="2" t="n">
         <v>91257</v>
       </c>
       <c r="E105" s="0" t="s">
@@ -9408,10 +9405,10 @@
       <c r="B106" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C106" s="3" t="n">
+      <c r="C106" s="2" t="n">
         <v>91967</v>
       </c>
-      <c r="D106" s="3" t="n">
+      <c r="D106" s="2" t="n">
         <v>92305</v>
       </c>
       <c r="E106" s="0" t="s">
@@ -9449,10 +9446,10 @@
       <c r="B107" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="3" t="n">
+      <c r="C107" s="2" t="n">
         <v>92815</v>
       </c>
-      <c r="D107" s="3" t="n">
+      <c r="D107" s="2" t="n">
         <v>94029</v>
       </c>
       <c r="E107" s="0" t="s">
@@ -9490,10 +9487,10 @@
       <c r="B108" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="3" t="n">
+      <c r="C108" s="2" t="n">
         <v>94058</v>
       </c>
-      <c r="D108" s="3" t="n">
+      <c r="D108" s="2" t="n">
         <v>95356</v>
       </c>
       <c r="E108" s="0" t="s">
@@ -9540,10 +9537,10 @@
       <c r="B109" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C109" s="3" t="n">
+      <c r="C109" s="2" t="n">
         <v>95470</v>
       </c>
-      <c r="D109" s="3" t="n">
+      <c r="D109" s="2" t="n">
         <v>96666</v>
       </c>
       <c r="E109" s="0" t="s">
@@ -9590,10 +9587,10 @@
       <c r="B110" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="3" t="n">
+      <c r="C110" s="2" t="n">
         <v>97551</v>
       </c>
-      <c r="D110" s="3" t="n">
+      <c r="D110" s="2" t="n">
         <v>97808</v>
       </c>
       <c r="E110" s="0" t="s">
@@ -9631,10 +9628,10 @@
       <c r="B111" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C111" s="3" t="n">
+      <c r="C111" s="2" t="n">
         <v>98307</v>
       </c>
-      <c r="D111" s="3" t="n">
+      <c r="D111" s="2" t="n">
         <v>99095</v>
       </c>
       <c r="E111" s="0" t="s">
@@ -9666,8 +9663,8 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
@@ -9676,10 +9673,10 @@
       <c r="B113" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C113" s="3" t="n">
+      <c r="C113" s="2" t="n">
         <v>99431</v>
       </c>
-      <c r="D113" s="3" t="n">
+      <c r="D113" s="2" t="n">
         <v>101452</v>
       </c>
       <c r="E113" s="0" t="s">
@@ -9750,10 +9747,10 @@
       <c r="B114" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C114" s="3" t="n">
+      <c r="C114" s="2" t="n">
         <v>101583</v>
       </c>
-      <c r="D114" s="3" t="n">
+      <c r="D114" s="2" t="n">
         <v>103160</v>
       </c>
       <c r="E114" s="0" t="s">
@@ -9809,10 +9806,10 @@
       <c r="B115" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C115" s="3" t="n">
+      <c r="C115" s="2" t="n">
         <v>103164</v>
       </c>
-      <c r="D115" s="3" t="n">
+      <c r="D115" s="2" t="n">
         <v>103967</v>
       </c>
       <c r="E115" s="0" t="s">
@@ -9862,10 +9859,10 @@
       <c r="B116" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C116" s="3" t="n">
+      <c r="C116" s="2" t="n">
         <v>103964</v>
       </c>
-      <c r="D116" s="3" t="n">
+      <c r="D116" s="2" t="n">
         <v>105064</v>
       </c>
       <c r="E116" s="0" t="s">
@@ -9918,10 +9915,10 @@
       <c r="B117" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C117" s="3" t="n">
+      <c r="C117" s="2" t="n">
         <v>105061</v>
       </c>
-      <c r="D117" s="3" t="n">
+      <c r="D117" s="2" t="n">
         <v>114558</v>
       </c>
       <c r="E117" s="0" t="s">
@@ -9974,10 +9971,10 @@
       <c r="B118" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C118" s="3" t="n">
+      <c r="C118" s="2" t="n">
         <v>114646</v>
       </c>
-      <c r="D118" s="3" t="n">
+      <c r="D118" s="2" t="n">
         <v>120753</v>
       </c>
       <c r="E118" s="0" t="s">
@@ -10027,10 +10024,10 @@
       <c r="B119" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C119" s="3" t="n">
+      <c r="C119" s="2" t="n">
         <v>120944</v>
       </c>
-      <c r="D119" s="3" t="n">
+      <c r="D119" s="2" t="n">
         <v>121903</v>
       </c>
       <c r="E119" s="0" t="s">
@@ -10080,10 +10077,10 @@
       <c r="B120" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C120" s="3" t="n">
+      <c r="C120" s="2" t="n">
         <v>122271</v>
       </c>
-      <c r="D120" s="3" t="n">
+      <c r="D120" s="2" t="n">
         <v>124073</v>
       </c>
       <c r="E120" s="0" t="s">
@@ -10130,10 +10127,10 @@
       <c r="B121" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C121" s="3" t="n">
+      <c r="C121" s="2" t="n">
         <v>124060</v>
       </c>
-      <c r="D121" s="3" t="n">
+      <c r="D121" s="2" t="n">
         <v>125862</v>
       </c>
       <c r="E121" s="0" t="s">
@@ -10183,10 +10180,10 @@
       <c r="B122" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C122" s="3" t="n">
+      <c r="C122" s="2" t="n">
         <v>125855</v>
       </c>
-      <c r="D122" s="3" t="n">
+      <c r="D122" s="2" t="n">
         <v>127135</v>
       </c>
       <c r="E122" s="0" t="s">
@@ -10233,10 +10230,10 @@
       <c r="B123" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C123" s="3" t="n">
+      <c r="C123" s="2" t="n">
         <v>127163</v>
       </c>
-      <c r="D123" s="3" t="n">
+      <c r="D123" s="2" t="n">
         <v>128494</v>
       </c>
       <c r="E123" s="0" t="s">
@@ -10283,8 +10280,8 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
@@ -10293,10 +10290,10 @@
       <c r="B125" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="3" t="n">
+      <c r="C125" s="2" t="n">
         <v>129152</v>
       </c>
-      <c r="D125" s="3" t="n">
+      <c r="D125" s="2" t="n">
         <v>129451</v>
       </c>
       <c r="E125" s="0" t="s">
@@ -10334,10 +10331,10 @@
       <c r="B126" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C126" s="3" t="n">
+      <c r="C126" s="2" t="n">
         <v>129686</v>
       </c>
-      <c r="D126" s="3" t="n">
+      <c r="D126" s="2" t="n">
         <v>131173</v>
       </c>
       <c r="E126" s="0" t="s">
@@ -10375,10 +10372,10 @@
       <c r="B127" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C127" s="3" t="n">
+      <c r="C127" s="2" t="n">
         <v>131258</v>
       </c>
-      <c r="D127" s="3" t="n">
+      <c r="D127" s="2" t="n">
         <v>132118</v>
       </c>
       <c r="E127" s="0" t="s">
@@ -10410,12 +10407,12 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
@@ -10424,10 +10421,10 @@
       <c r="B130" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C130" s="3" t="n">
+      <c r="C130" s="2" t="n">
         <v>133493</v>
       </c>
-      <c r="D130" s="3" t="n">
+      <c r="D130" s="2" t="n">
         <v>134506</v>
       </c>
       <c r="E130" s="0" t="s">
@@ -10459,12 +10456,12 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="2"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
@@ -10473,10 +10470,10 @@
       <c r="B133" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C133" s="3" t="n">
+      <c r="C133" s="2" t="n">
         <v>136027</v>
       </c>
-      <c r="D133" s="3" t="n">
+      <c r="D133" s="2" t="n">
         <v>136590</v>
       </c>
       <c r="E133" s="0" t="s">
@@ -10505,10 +10502,10 @@
       <c r="B134" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C134" s="3" t="n">
+      <c r="C134" s="2" t="n">
         <v>136599</v>
       </c>
-      <c r="D134" s="3" t="n">
+      <c r="D134" s="2" t="n">
         <v>136901</v>
       </c>
       <c r="E134" s="0" t="s">
@@ -10540,8 +10537,8 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="3"/>
-      <c r="D135" s="3"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
@@ -10550,10 +10547,10 @@
       <c r="B136" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C136" s="3" t="n">
+      <c r="C136" s="2" t="n">
         <v>137785</v>
       </c>
-      <c r="D136" s="3" t="n">
+      <c r="D136" s="2" t="n">
         <v>138369</v>
       </c>
       <c r="E136" s="0" t="s">
@@ -10585,8 +10582,8 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
@@ -10595,10 +10592,10 @@
       <c r="B138" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C138" s="3" t="n">
+      <c r="C138" s="2" t="n">
         <v>139407</v>
       </c>
-      <c r="D138" s="3" t="n">
+      <c r="D138" s="2" t="n">
         <v>140795</v>
       </c>
       <c r="E138" s="0" t="s">
@@ -10636,10 +10633,10 @@
       <c r="B139" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C139" s="3" t="n">
+      <c r="C139" s="2" t="n">
         <v>141123</v>
       </c>
-      <c r="D139" s="3" t="n">
+      <c r="D139" s="2" t="n">
         <v>141491</v>
       </c>
       <c r="E139" s="0" t="s">
@@ -10718,10 +10715,10 @@
       <c r="B141" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C141" s="3" t="n">
+      <c r="C141" s="2" t="n">
         <v>144423</v>
       </c>
-      <c r="D141" s="3" t="n">
+      <c r="D141" s="2" t="n">
         <v>145400</v>
       </c>
       <c r="E141" s="0" t="s">
@@ -10777,10 +10774,10 @@
       <c r="B142" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C142" s="3" t="n">
+      <c r="C142" s="2" t="n">
         <v>145850</v>
       </c>
-      <c r="D142" s="3" t="n">
+      <c r="D142" s="2" t="n">
         <v>147187</v>
       </c>
       <c r="E142" s="0" t="s">
@@ -10836,10 +10833,10 @@
       <c r="B143" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C143" s="3" t="n">
+      <c r="C143" s="2" t="n">
         <v>147426</v>
       </c>
-      <c r="D143" s="3" t="n">
+      <c r="D143" s="2" t="n">
         <v>148499</v>
       </c>
       <c r="E143" s="0" t="s">
@@ -10880,10 +10877,10 @@
       <c r="B144" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C144" s="3" t="n">
+      <c r="C144" s="2" t="n">
         <v>148818</v>
       </c>
-      <c r="D144" s="3" t="n">
+      <c r="D144" s="2" t="n">
         <v>151085</v>
       </c>
       <c r="E144" s="0" t="s">
@@ -10924,10 +10921,10 @@
       <c r="B145" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C145" s="3" t="n">
+      <c r="C145" s="2" t="n">
         <v>152772</v>
       </c>
-      <c r="D145" s="3" t="n">
+      <c r="D145" s="2" t="n">
         <v>153080</v>
       </c>
       <c r="E145" s="0" t="s">
@@ -10965,10 +10962,10 @@
       <c r="B146" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C146" s="3" t="n">
+      <c r="C146" s="2" t="n">
         <v>154116</v>
       </c>
-      <c r="D146" s="3" t="n">
+      <c r="D146" s="2" t="n">
         <v>154406</v>
       </c>
       <c r="E146" s="0" t="s">
@@ -11032,10 +11029,10 @@
       <c r="B148" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C148" s="3" t="n">
+      <c r="C148" s="2" t="n">
         <v>156089</v>
       </c>
-      <c r="D148" s="3" t="n">
+      <c r="D148" s="2" t="n">
         <v>156685</v>
       </c>
       <c r="E148" s="0" t="s">
@@ -12542,10 +12539,10 @@
       <c r="B181" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C181" s="3" t="n">
+      <c r="C181" s="2" t="n">
         <v>183153</v>
       </c>
-      <c r="D181" s="3" t="n">
+      <c r="D181" s="2" t="n">
         <v>183413</v>
       </c>
       <c r="E181" s="0" t="s">
@@ -12554,7 +12551,7 @@
       <c r="F181" s="0" t="s">
         <v>1107</v>
       </c>
-      <c r="G181" s="2" t="s">
+      <c r="G181" s="1" t="s">
         <v>1108</v>
       </c>
       <c r="H181" s="0" t="s">
@@ -14516,10 +14513,10 @@
       <c r="B226" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C226" s="3" t="n">
+      <c r="C226" s="2" t="n">
         <v>230496</v>
       </c>
-      <c r="D226" s="3" t="n">
+      <c r="D226" s="2" t="n">
         <v>230828</v>
       </c>
       <c r="E226" s="0" t="s">
@@ -14791,10 +14788,10 @@
       <c r="B233" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C233" s="3" t="n">
+      <c r="C233" s="2" t="n">
         <v>234393</v>
       </c>
-      <c r="D233" s="3" t="n">
+      <c r="D233" s="2" t="n">
         <v>234659</v>
       </c>
       <c r="E233" s="0" t="s">
@@ -15082,10 +15079,10 @@
       <c r="B241" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C241" s="3" t="n">
+      <c r="C241" s="2" t="n">
         <v>240747</v>
       </c>
-      <c r="D241" s="3" t="n">
+      <c r="D241" s="2" t="n">
         <v>241181</v>
       </c>
       <c r="E241" s="0" t="s">
@@ -15094,7 +15091,7 @@
       <c r="F241" s="0" t="s">
         <v>1551</v>
       </c>
-      <c r="G241" s="2" t="s">
+      <c r="G241" s="1" t="s">
         <v>1552</v>
       </c>
       <c r="H241" s="0" t="s">
@@ -15311,10 +15308,10 @@
       <c r="B246" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C246" s="3" t="n">
+      <c r="C246" s="2" t="n">
         <v>245028</v>
       </c>
-      <c r="D246" s="3" t="n">
+      <c r="D246" s="2" t="n">
         <v>245450</v>
       </c>
       <c r="E246" s="0" t="s">
@@ -15352,10 +15349,10 @@
       <c r="B247" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C247" s="3" t="n">
+      <c r="C247" s="2" t="n">
         <v>245497</v>
       </c>
-      <c r="D247" s="3" t="n">
+      <c r="D247" s="2" t="n">
         <v>245922</v>
       </c>
       <c r="E247" s="0" t="s">
@@ -15551,10 +15548,10 @@
       <c r="B252" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C252" s="3" t="n">
+      <c r="C252" s="2" t="n">
         <v>248897</v>
       </c>
-      <c r="D252" s="3" t="n">
+      <c r="D252" s="2" t="n">
         <v>249823</v>
       </c>
       <c r="E252" s="0" t="s">
@@ -16065,10 +16062,10 @@
       <c r="B263" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C263" s="3" t="n">
+      <c r="C263" s="2" t="n">
         <v>257761</v>
       </c>
-      <c r="D263" s="3" t="n">
+      <c r="D263" s="2" t="n">
         <v>258252</v>
       </c>
       <c r="E263" s="0" t="s">
@@ -16106,10 +16103,10 @@
       <c r="B264" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C264" s="3" t="n">
+      <c r="C264" s="2" t="n">
         <v>258295</v>
       </c>
-      <c r="D264" s="3" t="n">
+      <c r="D264" s="2" t="n">
         <v>259416</v>
       </c>
       <c r="E264" s="0" t="s">
@@ -16147,10 +16144,10 @@
       <c r="B265" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C265" s="3" t="n">
+      <c r="C265" s="2" t="n">
         <v>259704</v>
       </c>
-      <c r="D265" s="3" t="n">
+      <c r="D265" s="2" t="n">
         <v>259961</v>
       </c>
       <c r="E265" s="0" t="s">
@@ -16317,10 +16314,10 @@
       <c r="B269" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C269" s="3" t="n">
+      <c r="C269" s="2" t="n">
         <v>263477</v>
       </c>
-      <c r="D269" s="3" t="n">
+      <c r="D269" s="2" t="n">
         <v>264181</v>
       </c>
       <c r="E269" s="0" t="s">
@@ -16669,10 +16666,10 @@
       <c r="B277" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C277" s="3" t="n">
+      <c r="C277" s="2" t="n">
         <v>270025</v>
       </c>
-      <c r="D277" s="3" t="n">
+      <c r="D277" s="2" t="n">
         <v>270690</v>
       </c>
       <c r="E277" s="0" t="s">
@@ -16722,10 +16719,10 @@
       <c r="B278" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C278" s="3" t="n">
+      <c r="C278" s="2" t="n">
         <v>271571</v>
       </c>
-      <c r="D278" s="3" t="n">
+      <c r="D278" s="2" t="n">
         <v>272779</v>
       </c>
       <c r="E278" s="0" t="s">
@@ -16763,10 +16760,10 @@
       <c r="B279" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C279" s="3" t="n">
+      <c r="C279" s="2" t="n">
         <v>272906</v>
       </c>
-      <c r="D279" s="3" t="n">
+      <c r="D279" s="2" t="n">
         <v>273805</v>
       </c>
       <c r="E279" s="0" t="s">
@@ -16801,10 +16798,10 @@
       <c r="B280" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C280" s="3" t="n">
+      <c r="C280" s="2" t="n">
         <v>274868</v>
       </c>
-      <c r="D280" s="3" t="n">
+      <c r="D280" s="2" t="n">
         <v>275380</v>
       </c>
       <c r="E280" s="0" t="s">
@@ -16848,10 +16845,10 @@
       <c r="B281" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C281" s="3" t="n">
+      <c r="C281" s="2" t="n">
         <v>275721</v>
       </c>
-      <c r="D281" s="3" t="n">
+      <c r="D281" s="2" t="n">
         <v>276233</v>
       </c>
       <c r="E281" s="0" t="s">
@@ -16877,10 +16874,10 @@
       <c r="B282" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C282" s="3" t="n">
+      <c r="C282" s="2" t="n">
         <v>276399</v>
       </c>
-      <c r="D282" s="3" t="n">
+      <c r="D282" s="2" t="n">
         <v>276896</v>
       </c>
       <c r="E282" s="0" t="s">
@@ -16900,8 +16897,8 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="3"/>
-      <c r="D283" s="3"/>
+      <c r="C283" s="2"/>
+      <c r="D283" s="2"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
@@ -16910,10 +16907,10 @@
       <c r="B284" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C284" s="3" t="n">
+      <c r="C284" s="2" t="n">
         <v>277717</v>
       </c>
-      <c r="D284" s="3" t="n">
+      <c r="D284" s="2" t="n">
         <v>278112</v>
       </c>
       <c r="E284" s="0" t="s">
@@ -16939,10 +16936,10 @@
       <c r="B285" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C285" s="3" t="n">
+      <c r="C285" s="2" t="n">
         <v>278224</v>
       </c>
-      <c r="D285" s="3" t="n">
+      <c r="D285" s="2" t="n">
         <v>278520</v>
       </c>
       <c r="E285" s="0" t="s">
@@ -16971,10 +16968,10 @@
       <c r="B286" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C286" s="3" t="n">
+      <c r="C286" s="2" t="n">
         <v>278737</v>
       </c>
-      <c r="D286" s="3" t="n">
+      <c r="D286" s="2" t="n">
         <v>278916</v>
       </c>
       <c r="E286" s="0" t="s">
@@ -16997,8 +16994,8 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="3"/>
-      <c r="D287" s="3"/>
+      <c r="C287" s="2"/>
+      <c r="D287" s="2"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
@@ -17007,10 +17004,10 @@
       <c r="B288" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C288" s="3" t="n">
+      <c r="C288" s="2" t="n">
         <v>280889</v>
       </c>
-      <c r="D288" s="3" t="n">
+      <c r="D288" s="2" t="n">
         <v>281101</v>
       </c>
       <c r="E288" s="0" t="s">
@@ -17045,10 +17042,10 @@
       <c r="B289" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C289" s="3" t="n">
+      <c r="C289" s="2" t="n">
         <v>282211</v>
       </c>
-      <c r="D289" s="3" t="n">
+      <c r="D289" s="2" t="n">
         <v>283170</v>
       </c>
       <c r="E289" s="0" t="s">
@@ -17086,10 +17083,10 @@
       <c r="B290" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C290" s="3" t="n">
+      <c r="C290" s="2" t="n">
         <v>283170</v>
       </c>
-      <c r="D290" s="3" t="n">
+      <c r="D290" s="2" t="n">
         <v>284336</v>
       </c>
       <c r="E290" s="0" t="s">
@@ -17130,7 +17127,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B294" s="3" t="s">
+      <c r="B294" s="2" t="s">
         <v>1881</v>
       </c>
     </row>
@@ -17145,4 +17142,613 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A141"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>838</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>